<commit_message>
add normalization to the naive bayes classifier calculation, update the front end prediction page
</commit_message>
<xml_diff>
--- a/backend/data.xlsx
+++ b/backend/data.xlsx
@@ -16,28 +16,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="25">
   <si>
-    <t>Jenis Kelamin</t>
-  </si>
-  <si>
-    <t>Organisasi</t>
-  </si>
-  <si>
-    <t>Ekstrakurikuler</t>
-  </si>
-  <si>
-    <t>Sertifikasi Profesi</t>
-  </si>
-  <si>
-    <t>Nilai Akhir</t>
-  </si>
-  <si>
-    <t>Tempat Magang</t>
-  </si>
-  <si>
-    <t>Tempat Kerja</t>
-  </si>
-  <si>
-    <t>Durasi Mendapat Kerja dibawah 3 Bulan</t>
+    <t>jenisKelamin</t>
+  </si>
+  <si>
+    <t>organisasi</t>
+  </si>
+  <si>
+    <t>ekstrakurikuler</t>
+  </si>
+  <si>
+    <t>sertifikasiProfesi</t>
+  </si>
+  <si>
+    <t>nilaiAkhir</t>
+  </si>
+  <si>
+    <t>tempatMagang</t>
+  </si>
+  <si>
+    <t>tempatKerja</t>
+  </si>
+  <si>
+    <t>Durasi Mendapat Kerja</t>
   </si>
   <si>
     <t>Perempuan</t>

</xml_diff>

<commit_message>
feat: automate Excel header formatting, fix prediction errors, and update prediction page UI
Details:
- Implemented automatic header formatting for uploaded Excel files in the /upload endpoint.
- Fixed errors in the /predict endpoint to ensure consistent prediction results.
- Updated the prediction page to include a "Silahkan Dipilih" option for improved user experience.
</commit_message>
<xml_diff>
--- a/backend/data.xlsx
+++ b/backend/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="26">
   <si>
     <t>jenisKelamin</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Kompeten</t>
+  </si>
+  <si>
+    <t>Tidak Kompeten</t>
   </si>
   <si>
     <t>Sangat Baik</t>
@@ -446,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -492,16 +495,16 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -518,16 +521,16 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -544,16 +547,16 @@
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -570,16 +573,16 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -596,16 +599,16 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -622,16 +625,16 @@
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -648,16 +651,16 @@
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -674,16 +677,16 @@
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -694,7 +697,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
@@ -703,10 +706,10 @@
         <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H10" t="s">
         <v>24</v>
@@ -726,15 +729,925 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" t="s">
+        <v>20</v>
+      </c>
+      <c r="H41" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" t="s">
+        <v>20</v>
+      </c>
+      <c r="H42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43" t="s">
+        <v>22</v>
+      </c>
+      <c r="H43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" t="s">
+        <v>20</v>
+      </c>
+      <c r="H44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" t="s">
+        <v>23</v>
+      </c>
+      <c r="H45" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" t="s">
+        <v>23</v>
+      </c>
+      <c r="H46" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>